<commit_message>
upgrade backend test flow quality
</commit_message>
<xml_diff>
--- a/backend/הסטוריית נתמכים.xlsx
+++ b/backend/הסטוריית נתמכים.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\shalom\gmah\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EBE846-39DC-472F-9F59-D56EA6451277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D20144-3F44-425F-ABB9-81EA5FC2D1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>שם מלא</t>
   </si>
@@ -50,6 +50,27 @@
   </si>
   <si>
     <t>סיבה</t>
+  </si>
+  <si>
+    <t>שפרינצק</t>
+  </si>
+  <si>
+    <t>012-3456789</t>
+  </si>
+  <si>
+    <t>987-6543210</t>
+  </si>
+  <si>
+    <t>רווחה</t>
+  </si>
+  <si>
+    <t>הוסרה מהגמח</t>
+  </si>
+  <si>
+    <t>27 יולי 2023</t>
+  </si>
+  <si>
+    <t>לא עונה לטלפון</t>
   </si>
 </sst>
 </file>
@@ -555,7 +576,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" x14ac:dyDescent="0.45"/>
@@ -571,8 +592,8 @@
     <col min="11" max="11" width="8.80859375" style="4" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.1875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="30" width="8.80859375" style="4" customWidth="1"/>
-    <col min="31" max="16384" width="8.80859375" style="4"/>
+    <col min="14" max="32" width="8.80859375" style="4" customWidth="1"/>
+    <col min="33" max="16384" width="8.80859375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -608,16 +629,36 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>